<commit_message>
add new exercises, various updates
- updated anki decks/wordlists to reflect the changes made below.
- updated lesson-4/vocab-7 & 8; stand alone number --> XX day of the month. (#143)
- updated lesson-11/vocab-7; "exercise" --> "practice; (an) exercise" (#142)
- added the following exercises.

# Lesson 22 (3rd ed.)
- Kanji Practice: Stroke Order
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-4.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-4.xlsx
@@ -1432,7 +1432,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>first day of the month</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1444,7 +1444,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>second day of the month</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1456,7 +1456,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>third day of the month</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1468,7 +1468,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>fourth day of the month</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1480,7 +1480,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>fifth day of the month</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>sixth day of the month</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1504,7 +1504,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>seventh day of the month</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1516,7 +1516,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>eighth day of the month</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1528,7 +1528,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>ninth day of the month</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>tenth day of the month</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>eleventh day of the month</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1564,7 +1564,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>twelth day of the month</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1576,7 +1576,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>thirteenth day of the month</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>fourteenth day of the month</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1600,7 +1600,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>fifteenth day of the month</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1612,7 +1612,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>sixteenth day of the month</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1624,7 +1624,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>seventeenth day of the month</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -1636,7 +1636,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>eighteenth day of the month</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -1648,7 +1648,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>nineteenth day of the month</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1660,7 +1660,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>twentieth day of the month</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -1672,7 +1672,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>twenty-first day of the month</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -1684,7 +1684,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>twenty-second day of the month</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -1696,7 +1696,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>twenty-third day of the month</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -1708,7 +1708,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>twenty-fourth day of the month</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1720,7 +1720,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>twenty-fifth day of the month</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1732,7 +1732,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>twenty-sixth day of the month</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -1744,7 +1744,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>twenty-seventh day of the month</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -1756,7 +1756,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>twenty-eighth day of the month</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1768,7 +1768,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>twenty-ninth day of the month</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1780,7 +1780,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>thirtieth day of the month</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -1792,7 +1792,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>thiry-first day of the month</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">

</xml_diff>